<commit_message>
Enemies: Fixed some missing data and added default values for stats.
</commit_message>
<xml_diff>
--- a/Research/Tests/DownscalingNew.xlsx
+++ b/Research/Tests/DownscalingNew.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Attribute" sheetId="2" r:id="rId1"/>
     <sheet name="Graph Gear Attributes" sheetId="3" r:id="rId2"/>
     <sheet name="Data Attributes" sheetId="1" r:id="rId3"/>
     <sheet name="Retaliation" sheetId="4" r:id="rId4"/>
+    <sheet name="Weapon" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -201,7 +202,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t>Known facts:</t>
   </si>
@@ -252,6 +253,45 @@
   </si>
   <si>
     <t>Attributes</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t>Fine</t>
+  </si>
+  <si>
+    <t>Masterwork</t>
+  </si>
+  <si>
+    <t>Rare</t>
+  </si>
+  <si>
+    <t>Exotic</t>
+  </si>
+  <si>
+    <t>Ascended</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Armor</t>
+  </si>
+  <si>
+    <t>Damage</t>
+  </si>
+  <si>
+    <t>Coeff</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Wep</t>
+  </si>
+  <si>
+    <t>Expected</t>
   </si>
 </sst>
 </file>
@@ -337,7 +377,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -610,7 +649,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="70" formatCode="0.00%">
-                  <c:v>#N/A</c:v>
+                  <c:v>0.9998530862383781</c:v>
                 </c:pt>
                 <c:pt idx="71" formatCode="0.00%">
                   <c:v>1.0001564978793347</c:v>
@@ -881,7 +920,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="70" formatCode="0.00%">
-                  <c:v>#N/A</c:v>
+                  <c:v>0.9998530862383781</c:v>
                 </c:pt>
                 <c:pt idx="71" formatCode="0.00%">
                   <c:v>1.0001564978793347</c:v>
@@ -1152,7 +1191,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="70" formatCode="0.00%">
-                  <c:v>#N/A</c:v>
+                  <c:v>0.9998530862383781</c:v>
                 </c:pt>
                 <c:pt idx="71" formatCode="0.00%">
                   <c:v>1.0001564978793347</c:v>
@@ -1423,7 +1462,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="70" formatCode="0.00%">
-                  <c:v>#N/A</c:v>
+                  <c:v>0.9998530862383781</c:v>
                 </c:pt>
                 <c:pt idx="71" formatCode="0.00%">
                   <c:v>1.0001564978793347</c:v>
@@ -1694,7 +1733,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="70" formatCode="0.00%">
-                  <c:v>#N/A</c:v>
+                  <c:v>0.9998530862383781</c:v>
                 </c:pt>
                 <c:pt idx="71" formatCode="0.00%">
                   <c:v>1.0001564978793347</c:v>
@@ -1965,7 +2004,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="70" formatCode="0.00%">
-                  <c:v>#N/A</c:v>
+                  <c:v>0.9998530862383781</c:v>
                 </c:pt>
                 <c:pt idx="71" formatCode="0.00%">
                   <c:v>1.0001564978793347</c:v>
@@ -2232,7 +2271,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="70" formatCode="0.00%">
-                  <c:v>#N/A</c:v>
+                  <c:v>0.9998530862383781</c:v>
                 </c:pt>
                 <c:pt idx="71" formatCode="0.00%">
                   <c:v>1.0001564978793347</c:v>
@@ -2499,7 +2538,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="70" formatCode="0.00%">
-                  <c:v>#N/A</c:v>
+                  <c:v>0.9998530862383781</c:v>
                 </c:pt>
                 <c:pt idx="71" formatCode="0.00%">
                   <c:v>1.0001564978793347</c:v>
@@ -2766,7 +2805,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="70" formatCode="0.00%">
-                  <c:v>#N/A</c:v>
+                  <c:v>0.9998530862383781</c:v>
                 </c:pt>
                 <c:pt idx="71" formatCode="0.00%">
                   <c:v>1.0001564978793347</c:v>
@@ -3033,7 +3072,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="70" formatCode="0.00%">
-                  <c:v>#N/A</c:v>
+                  <c:v>0.9998530862383781</c:v>
                 </c:pt>
                 <c:pt idx="71" formatCode="0.00%">
                   <c:v>1.0001564978793347</c:v>
@@ -3300,7 +3339,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="70" formatCode="0.00%">
-                  <c:v>#N/A</c:v>
+                  <c:v>0.9998530862383781</c:v>
                 </c:pt>
                 <c:pt idx="71" formatCode="0.00%">
                   <c:v>1.0001564978793347</c:v>
@@ -3374,7 +3413,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -3613,7 +3651,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="70" formatCode="0.00%">
-                  <c:v>#N/A</c:v>
+                  <c:v>0.9998530862383781</c:v>
                 </c:pt>
                 <c:pt idx="71" formatCode="0.00%">
                   <c:v>1.0001564978793347</c:v>
@@ -3655,11 +3693,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="325397712"/>
-        <c:axId val="325389552"/>
+        <c:axId val="337797248"/>
+        <c:axId val="337797792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="325397712"/>
+        <c:axId val="337797248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3702,12 +3740,12 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="325389552"/>
+        <c:crossAx val="337797792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="325389552"/>
+        <c:axId val="337797792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3758,7 +3796,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="325397712"/>
+        <c:crossAx val="337797248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4151,7 +4189,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>#N/A</c:v>
+                  <c:v>0.77488614183474303</c:v>
                 </c:pt>
                 <c:pt idx="68">
                   <c:v>0.81912817176317498</c:v>
@@ -4193,11 +4231,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="325394448"/>
-        <c:axId val="325394992"/>
+        <c:axId val="337796160"/>
+        <c:axId val="337796704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="325394448"/>
+        <c:axId val="337796160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4240,12 +4278,12 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="325394992"/>
+        <c:crossAx val="337796704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="325394992"/>
+        <c:axId val="337796704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4296,7 +4334,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="325394448"/>
+        <c:crossAx val="337796160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4360,7 +4398,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4919,11 +4956,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="557173744"/>
-        <c:axId val="557166672"/>
+        <c:axId val="339922704"/>
+        <c:axId val="339927056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="557173744"/>
+        <c:axId val="339922704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4966,7 +5003,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="557166672"/>
+        <c:crossAx val="339927056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4974,7 +5011,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="557166672"/>
+        <c:axId val="339927056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5025,7 +5062,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="557173744"/>
+        <c:crossAx val="339922704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5039,7 +5076,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7165,7 +7201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -8413,8 +8449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9595,19 +9631,19 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>0</v>
+        <v>1966</v>
       </c>
       <c r="B71">
         <f t="shared" ca="1" si="2"/>
-        <v>-775</v>
-      </c>
-      <c r="C71" s="1" t="e">
+        <v>1191</v>
+      </c>
+      <c r="C71" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D71" s="1" t="e">
+        <v>0.77488614183474303</v>
+      </c>
+      <c r="D71" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>#N/A</v>
+        <v>0.9998530862383781</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -10851,7 +10887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
@@ -12099,4 +12135,354 @@
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1">
+        <v>80</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1">
+        <v>542</v>
+      </c>
+      <c r="O1">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>551</v>
+      </c>
+      <c r="C2">
+        <v>609</v>
+      </c>
+      <c r="D2">
+        <f>(B2+C2)/2</f>
+        <v>580</v>
+      </c>
+      <c r="E2">
+        <f>D5/D2</f>
+        <v>1.4551724137931035</v>
+      </c>
+      <c r="G2">
+        <v>253</v>
+      </c>
+      <c r="H2">
+        <v>279</v>
+      </c>
+      <c r="I2">
+        <f>(G2+H2)/2</f>
+        <v>266</v>
+      </c>
+      <c r="J2">
+        <f>I5/I2</f>
+        <v>1.4755639097744362</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2">
+        <v>1.8</v>
+      </c>
+      <c r="O2">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>690</v>
+      </c>
+      <c r="C3">
+        <v>762</v>
+      </c>
+      <c r="D3">
+        <f>(B3+C3)/2</f>
+        <v>726</v>
+      </c>
+      <c r="L3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3">
+        <v>497</v>
+      </c>
+      <c r="O3">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>745</v>
+      </c>
+      <c r="C4">
+        <v>823</v>
+      </c>
+      <c r="D4">
+        <f>(B4+C4)/2</f>
+        <v>784</v>
+      </c>
+      <c r="E4">
+        <f>D5/D4</f>
+        <v>1.0765306122448979</v>
+      </c>
+      <c r="G4">
+        <v>344</v>
+      </c>
+      <c r="H4">
+        <v>380</v>
+      </c>
+      <c r="I4">
+        <f>(G4+H4)/2</f>
+        <v>362</v>
+      </c>
+      <c r="J4">
+        <f>I5/I4</f>
+        <v>1.0842541436464088</v>
+      </c>
+      <c r="L4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4">
+        <v>624</v>
+      </c>
+      <c r="O4">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>802</v>
+      </c>
+      <c r="C5">
+        <v>886</v>
+      </c>
+      <c r="D5">
+        <f>(B5+C5)/2</f>
+        <v>844</v>
+      </c>
+      <c r="E5">
+        <f>D7/D5</f>
+        <v>1.1848341232227488</v>
+      </c>
+      <c r="G5">
+        <v>373</v>
+      </c>
+      <c r="H5">
+        <v>412</v>
+      </c>
+      <c r="I5">
+        <f>(G5+H5)/2</f>
+        <v>392.5</v>
+      </c>
+      <c r="L5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5">
+        <f>M1/M2/M3*M4</f>
+        <v>378.05499664654587</v>
+      </c>
+      <c r="O5">
+        <f>O1/O2/O3*O4</f>
+        <v>289.2433537832311</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>905</v>
+      </c>
+      <c r="C6">
+        <v>1000</v>
+      </c>
+      <c r="D6">
+        <f>(B6+C6)/2</f>
+        <v>952.5</v>
+      </c>
+      <c r="E6">
+        <f>D7/D6</f>
+        <v>1.0498687664041995</v>
+      </c>
+      <c r="L6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6">
+        <f>G5*E5</f>
+        <v>441.94312796208533</v>
+      </c>
+      <c r="O6">
+        <f>K5*G5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>950</v>
+      </c>
+      <c r="C7">
+        <v>1050</v>
+      </c>
+      <c r="D7">
+        <f>(B7+C7)/2</f>
+        <v>1000</v>
+      </c>
+      <c r="M7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>62</v>
+      </c>
+      <c r="L10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M10">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>253</v>
+      </c>
+      <c r="C11">
+        <v>279</v>
+      </c>
+      <c r="D11">
+        <f>(B11+C11)/2</f>
+        <v>266</v>
+      </c>
+      <c r="E11">
+        <f>D14/D11</f>
+        <v>2.5432330827067671</v>
+      </c>
+      <c r="L11" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>27</v>
+      </c>
+      <c r="M12">
+        <v>2482</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>597</v>
+      </c>
+      <c r="C13">
+        <v>659</v>
+      </c>
+      <c r="D13">
+        <f>(B13+C13)/2</f>
+        <v>628</v>
+      </c>
+      <c r="E13">
+        <f>D14/D13</f>
+        <v>1.0772292993630572</v>
+      </c>
+      <c r="L13" t="s">
+        <v>24</v>
+      </c>
+      <c r="M13">
+        <v>2597</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>643</v>
+      </c>
+      <c r="C14">
+        <v>710</v>
+      </c>
+      <c r="D14">
+        <f>(B14+C14)/2</f>
+        <v>676.5</v>
+      </c>
+      <c r="E14">
+        <f>D15/D14</f>
+        <v>1.1308203991130821</v>
+      </c>
+      <c r="L14" t="s">
+        <v>28</v>
+      </c>
+      <c r="M14">
+        <f>M10/M11/M12*M13</f>
+        <v>948.67579908675793</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>727</v>
+      </c>
+      <c r="C15">
+        <v>803</v>
+      </c>
+      <c r="D15">
+        <f>(B15+C15)/2</f>
+        <v>765</v>
+      </c>
+      <c r="L15" t="s">
+        <v>29</v>
+      </c>
+      <c r="M15">
+        <f>I14*E14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>